<commit_message>
update account update, delete
</commit_message>
<xml_diff>
--- a/DRRMOFingerprintApp/Document/Registration-Form.xlsx
+++ b/DRRMOFingerprintApp/Document/Registration-Form.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Republic of the Philippines</t>
   </si>
@@ -200,13 +200,19 @@
   </si>
   <si>
     <t>OFFICE NAME</t>
+  </si>
+  <si>
+    <t>PERSON ID #</t>
+  </si>
+  <si>
+    <t>For DRRMO Processor ONLY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,13 +273,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="18">
@@ -467,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -628,33 +645,42 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1856,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1867,70 +1893,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
     </row>
     <row r="5" spans="1:10" ht="18.75">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>32</v>
       </c>
+      <c r="H7" s="83" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75">
+      <c r="H8" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="78"/>
+      <c r="J8" s="79"/>
     </row>
     <row r="9" spans="1:10" ht="15.75">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="H9" s="80"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="82"/>
     </row>
     <row r="10" spans="1:10" ht="23.1" customHeight="1">
       <c r="A10" s="2" t="s">
@@ -1948,25 +1987,25 @@
     </row>
     <row r="11" spans="1:10" ht="23.1" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70" t="s">
+      <c r="C11" s="68"/>
+      <c r="D11" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70" t="s">
+      <c r="E11" s="68"/>
+      <c r="F11" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="70"/>
+      <c r="G11" s="68"/>
       <c r="H11" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="70" t="s">
+      <c r="I11" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="71"/>
+      <c r="J11" s="76"/>
     </row>
     <row r="12" spans="1:10" ht="23.1" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -2008,11 +2047,11 @@
       <c r="C14" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="75"/>
-      <c r="F14" s="76"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="5" t="s">
         <v>18</v>
       </c>
@@ -2199,10 +2238,10 @@
         <v>49</v>
       </c>
       <c r="G26" s="13"/>
-      <c r="H26" s="70" t="s">
+      <c r="H26" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="I26" s="70"/>
+      <c r="I26" s="68"/>
       <c r="J26" s="40" t="s">
         <v>51</v>
       </c>
@@ -2258,20 +2297,20 @@
         <v>55</v>
       </c>
       <c r="B30" s="24"/>
-      <c r="C30" s="72" t="s">
+      <c r="C30" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="72"/>
-      <c r="E30" s="73"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="70"/>
       <c r="F30" s="64" t="s">
         <v>52</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="72" t="s">
+      <c r="H30" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="I30" s="72"/>
-      <c r="J30" s="73"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="70"/>
     </row>
     <row r="31" spans="1:10" ht="23.1" customHeight="1">
       <c r="A31" s="47" t="s">
@@ -2383,18 +2422,18 @@
     <row r="42" spans="1:10" ht="23.1" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="H30:J30"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>